<commit_message>
Updated JPN model - 2025-08-27 11:43
</commit_message>
<xml_diff>
--- a/VerveStacks_JPN/SuppXLS/Scen_advanced_features.xlsx
+++ b/VerveStacks_JPN/SuppXLS/Scen_advanced_features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1B8BBA-9FA0-4608-9904-2A92EA38D7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824B08BC-82CE-42B4-80F3-1F3B80C4BED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{22AE2797-EE70-457C-AC96-4BB7B6BD4E04}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{22AE2797-EE70-457C-AC96-4BB7B6BD4E04}"/>
   </bookViews>
   <sheets>
     <sheet name="veda input" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="249">
   <si>
     <t>ACT_MINLD</t>
   </si>
@@ -2762,6 +2762,9 @@
   </si>
   <si>
     <t>coal</t>
+  </si>
+  <si>
+    <t>Nuclear P</t>
   </si>
 </sst>
 </file>
@@ -3246,7 +3249,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F77616-F3F2-4CAD-9718-D78F2778A52A}">
   <dimension ref="B2:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -4073,7 +4078,7 @@
         <v>0.1</v>
       </c>
       <c r="H17" t="s">
-        <v>5</v>
+        <v>248</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>83</v>
@@ -4090,7 +4095,7 @@
       </c>
       <c r="P17" t="str">
         <f t="shared" si="0"/>
-        <v>Nuclear</v>
+        <v>Nuclear P</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="3"/>
@@ -5297,7 +5302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B99335-61C3-404F-89AE-B281012B672E}">
   <dimension ref="B2:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>